<commit_message>
CMC curve making done and report started
</commit_message>
<xml_diff>
--- a/Identity/CMC Graph.xlsx
+++ b/Identity/CMC Graph.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayan\Desktop\Final Project\Identity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C9A79347-82E6-409D-9D2E-B597D43346DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAC4A3-E60E-49F7-9BE5-6BCC0DCF75D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMC Graph" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -5090,7 +5090,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8687,612 +8687,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>CMC upto rank 100</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="9525" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'CMC Graph'!$I$2:$I$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>44.880980000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>47.083359000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47.321454600000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47.321454600000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50.892888400000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>51.130983200000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>51.190507000000004</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>51.250030800000005</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>51.726221800000005</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>51.726221800000005</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>51.845269800000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>51.845269800000004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>51.845269800000004</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>52.023841600000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>52.023841600000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>52.142889600000004</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>52.202413400000005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>52.202413400000005</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>52.202413400000005</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>52.261937200000006</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>52.261937200000006</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>52.261937200000006</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>52.261937200000006</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>52.261937200000006</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>52.380984800000007</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>52.440508600000008</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>52.440508600000008</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>52.440508600000008</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>52.440508600000008</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>52.500032400000009</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>52.500032400000009</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>52.500032400000009</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>52.85717540000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>52.85717540000001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>52.85717540000001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>52.85717540000001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>52.916699200000011</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>52.916699200000011</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>52.916699200000011</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>52.916699200000011</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>53.035746800000013</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>53.095270600000013</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>53.095270600000013</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>53.154794400000014</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>53.333365400000012</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53.333365400000012</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.392889200000013</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>53.452413000000014</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>53.452413000000014</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>53.452413000000014</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>53.452413000000014</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>53.511936800000015</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>53.750031800000016</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>53.750031800000016</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>53.809555600000017</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>53.869079400000018</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>53.869079400000018</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>53.869079400000018</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>53.869079400000018</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>53.869079400000018</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>54.285746400000015</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>54.345270200000016</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>54.583365200000017</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>54.583365200000017</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>54.583365200000017</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>54.642889000000018</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>54.642889000000018</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>54.642889000000018</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>54.702412800000019</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>54.702412800000019</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>54.702412800000019</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>54.821460400000021</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>55.000031400000019</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>55.119079400000018</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>55.178603200000019</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>55.178603200000019</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>55.297651200000018</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>55.297651200000018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-224E-4737-B024-77D494A87FB8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="654458448"/>
-        <c:axId val="654455824"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="654458448"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="654455824"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="654455824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="44"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="654458448"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9534,46 +8928,6 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13127,508 +12481,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -13889,59 +12741,21 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="24" name="Chart 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F87CD2FD-E454-46D3-B728-C36F42AD90B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1681" totalsRowShown="0">
-  <autoFilter ref="A1:E1681"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E1681" totalsRowShown="0">
+  <autoFilter ref="A1:E1681" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:E1681">
     <sortCondition ref="B1:B1681"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name=" "/>
-    <tableColumn id="3" name="Frequency in fused tables"/>
-    <tableColumn id="4" name="Percentage"/>
-    <tableColumn id="5" name="Sum" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name=" "/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Frequency in fused tables"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Percentage"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Sum" dataDxfId="1">
       <calculatedColumnFormula>IF(B2=B1,"",SUMIF(B:B,B2,D:D))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13950,14 +12764,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="G1:I544" totalsRowShown="0">
-  <autoFilter ref="G1:I544"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="G1:I544" totalsRowShown="0">
+  <autoFilter ref="G1:I544" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Max Rank" dataDxfId="0"/>
-    <tableColumn id="2" name="Sum">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Max Rank" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Sum">
       <calculatedColumnFormula>SUMPRODUCT(($B$2:$B$1681=G2)*$D$2:$D$1681)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Cumulative">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cumulative">
       <calculatedColumnFormula>SUM(I1,H2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14261,11 +13075,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1681"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A535" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G544" sqref="G544:I544"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29208,7 +28022,7 @@
         <v>514</v>
       </c>
       <c r="H515">
-        <f t="shared" ref="H515:H578" si="26">SUMPRODUCT(($B$2:$B$1681=G515)*$D$2:$D$1681)</f>
+        <f t="shared" ref="H515:H544" si="26">SUMPRODUCT(($B$2:$B$1681=G515)*$D$2:$D$1681)</f>
         <v>0.119048</v>
       </c>
       <c r="I515">
@@ -50535,7 +49349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>